<commit_message>
comit all connect Nhibernate dapper
</commit_message>
<xml_diff>
--- a/calendar.xlsx
+++ b/calendar.xlsx
@@ -1,20 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\THUCTAP-SOFTDREAM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03AF6B9D-CAFB-4ECB-8E45-97556FF03764}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E17C6696-12F9-4691-93A9-C3343B26E6FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{195AFB05-C4E2-4473-9BE1-1B84F1A2600F}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{195AFB05-C4E2-4473-9BE1-1B84F1A2600F}"/>
   </bookViews>
   <sheets>
     <sheet name="Weerk 1" sheetId="1" r:id="rId1"/>
     <sheet name="Week 2" sheetId="2" r:id="rId2"/>
+    <sheet name="Week3" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet2" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="18">
   <si>
     <t>Họ và tên</t>
   </si>
@@ -531,8 +533,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3986B02D-6D51-4C77-8873-1474D505E82B}">
   <dimension ref="A1:G8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.8" x14ac:dyDescent="0.3"/>
@@ -661,13 +663,13 @@
   <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.5" customWidth="1"/>
-    <col min="2" max="2" width="12.19921875" customWidth="1"/>
+    <col min="2" max="2" width="14.796875" customWidth="1"/>
     <col min="3" max="4" width="10.8984375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8.09765625" customWidth="1"/>
     <col min="6" max="7" width="10.8984375" bestFit="1" customWidth="1"/>
@@ -814,4 +816,178 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7F38778-C55A-47B8-9679-5101A84AEEC2}">
+  <dimension ref="A1:G9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="23" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.8984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.8984375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.8984375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+    </row>
+    <row r="2" spans="1:7" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+    </row>
+    <row r="3" spans="1:7" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+    </row>
+    <row r="4" spans="1:7" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" s="5">
+        <v>45362</v>
+      </c>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F4" s="5">
+        <v>45731</v>
+      </c>
+      <c r="G4" s="1"/>
+    </row>
+    <row r="5" spans="1:7" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+    </row>
+    <row r="6" spans="1:7" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="A6" s="2"/>
+      <c r="B6" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="A7" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G7" s="6"/>
+    </row>
+    <row r="8" spans="1:7" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="A8" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G8" s="6"/>
+    </row>
+    <row r="9" spans="1:7" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED9EBB2E-E54A-4DDD-8951-641F0899D8AB}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J29" sqref="J29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>